<commit_message>
merge some 2015 using Gavin's code; start to run analyses
</commit_message>
<xml_diff>
--- a/data/england_lookup/UK city centres w lsoa_codes.xlsx
+++ b/data/england_lookup/UK city centres w lsoa_codes.xlsx
@@ -1259,14 +1259,16 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="38.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="27.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5546875" hidden="1" customWidth="1"/>
     <col min="15" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1810,10 +1812,10 @@
       <c r="P11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="Q11" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="R11" s="4" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>